<commit_message>
adjust limits to use equal, and add code display on blood sugar.
</commit_message>
<xml_diff>
--- a/docs/CodeSystem-CPM.xlsx
+++ b/docs/CodeSystem-CPM.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.2.6-beta</t>
+    <t>0.2.7-beta</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2021-09-09T10:21:32-05:00</t>
+    <t>2021-09-14T11:10:08-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
add explicit Apple examples
</commit_message>
<xml_diff>
--- a/docs/CodeSystem-CPM.xlsx
+++ b/docs/CodeSystem-CPM.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-10-28T12:50:39-05:00</t>
+    <t>2022-11-17T12:54:43-06:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -138,7 +138,7 @@
     <t>Definition</t>
   </si>
   <si>
-    <t>1e11b692-1898-4351-a7c5-428f61c91817"</t>
+    <t>1e11b692-1898-4351-a7c5-428f61c91817</t>
   </si>
   <si>
     <t>MobileKidney</t>

</xml_diff>